<commit_message>
folders and symbols now render
</commit_message>
<xml_diff>
--- a/13-05-2025.xlsx
+++ b/13-05-2025.xlsx
@@ -7526,6 +7526,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -7553,12 +7559,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -7649,7 +7649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7657,44 +7657,47 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
@@ -7703,7 +7706,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8018,50 +8021,50 @@
     <col min="3" max="3" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="18" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="19" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
     <col min="22" max="22" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="23" max="23" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="24" max="24" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="26" max="26" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="27" max="27" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
     <col min="28" max="28" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="29" max="29" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="30" max="30" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="32" max="32" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="33" max="33" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
     <col min="34" max="34" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="35" max="35" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="36" max="36" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="38" max="38" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="39" max="39" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
     <col min="40" max="40" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="41" max="41" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="42" max="42" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="44" max="44" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="45" max="45" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
     <col min="46" max="46" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="47" max="47" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="48" max="48" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="50" max="50" style="16" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="51" max="51" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
     <col min="52" max="52" style="16" width="23.433571428571426" customWidth="1" bestFit="1"/>
@@ -8069,7 +8072,7 @@
     <col min="54" max="54" style="16" width="20.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -8125,7 +8128,7 @@
       <c r="BA1" s="2"/>
       <c r="BB1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -8181,7 +8184,7 @@
       <c r="BA2" s="2"/>
       <c r="BB2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>